<commit_message>
Update results with SCCLaC, CVSCC, and MOWOG8 events.
</commit_message>
<xml_diff>
--- a/2021/com-20210620.xlsx
+++ b/2021/com-20210620.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrye/personal/mac/results/2021/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC2E88A-F972-D549-9233-7980C892BB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6315" yWindow="-30" windowWidth="15060" windowHeight="7650"/>
+    <workbookView xWindow="13180" yWindow="500" windowWidth="16860" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -189,9 +195,6 @@
     <t xml:space="preserve"> GORDON HANDELAND</t>
   </si>
   <si>
-    <t xml:space="preserve"> XS-A</t>
-  </si>
-  <si>
     <t xml:space="preserve"> STU</t>
   </si>
   <si>
@@ -210,23 +213,26 @@
     <t xml:space="preserve"> DAVE FARRELL</t>
   </si>
   <si>
-    <t xml:space="preserve"> KYLE GREEN</t>
-  </si>
-  <si>
     <t xml:space="preserve"> GS</t>
   </si>
   <si>
     <t xml:space="preserve"> ROBIN NEWBORG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> KYLE GREENE</t>
+  </si>
+  <si>
+    <t>XA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -555,30 +561,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -595,7 +601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>32</v>
@@ -608,14 +614,14 @@
       </c>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -626,7 +632,7 @@
         <v>60.218000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>22</v>
       </c>
@@ -637,7 +643,7 @@
         <v>60.960999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -648,7 +654,7 @@
         <v>61.473999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -659,7 +665,7 @@
         <v>62.268000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>22</v>
       </c>
@@ -670,11 +676,11 @@
         <v>64.894000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>52</v>
       </c>
@@ -685,10 +691,10 @@
         <v>59.512999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -699,7 +705,7 @@
         <v>61.298000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>9</v>
       </c>
@@ -710,7 +716,7 @@
         <v>63.136000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -721,7 +727,7 @@
         <v>63.722000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -732,7 +738,7 @@
         <v>63.764000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -743,11 +749,11 @@
         <v>75.792000000000002</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C17"/>
       <c r="D17"/>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -758,11 +764,11 @@
         <v>63.151000000000003</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C19"/>
       <c r="D19"/>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>30</v>
       </c>
@@ -773,10 +779,10 @@
         <v>80.744</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>29</v>
       </c>
@@ -787,7 +793,7 @@
         <v>60.109000000000002</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>29</v>
       </c>
@@ -798,7 +804,7 @@
         <v>60.122</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>29</v>
       </c>
@@ -809,10 +815,10 @@
         <v>61.075000000000003</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>19</v>
       </c>
@@ -823,7 +829,7 @@
         <v>59.034999999999997</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>19</v>
       </c>
@@ -834,7 +840,7 @@
         <v>59.265000000000001</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>19</v>
       </c>
@@ -845,7 +851,7 @@
         <v>59.478999999999999</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>19</v>
       </c>
@@ -856,11 +862,11 @@
         <v>63.024999999999999</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C30"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>17</v>
       </c>
@@ -871,7 +877,7 @@
         <v>64.040000000000006</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>17</v>
       </c>
@@ -882,10 +888,10 @@
         <v>65.677000000000007</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>20</v>
       </c>
@@ -896,7 +902,7 @@
         <v>61.168999999999997</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>20</v>
       </c>
@@ -907,7 +913,7 @@
         <v>63.197000000000003</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>20</v>
       </c>
@@ -918,12 +924,12 @@
         <v>63.923999999999999</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
         <v>36</v>
@@ -932,41 +938,41 @@
         <v>60.072000000000003</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C39"/>
       <c r="D39"/>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" t="s">
         <v>57</v>
-      </c>
-      <c r="C40" t="s">
-        <v>58</v>
       </c>
       <c r="D40">
         <v>62.892000000000003</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C41"/>
       <c r="D41"/>
     </row>
-    <row r="42" spans="2:4">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>28</v>
       </c>
       <c r="C42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D42">
         <v>61.344999999999999</v>
       </c>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C43"/>
       <c r="D43"/>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>31</v>
       </c>
@@ -977,13 +983,13 @@
         <v>61.662999999999997</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C45"/>
       <c r="D45"/>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C46" t="s">
         <v>35</v>
@@ -992,11 +998,11 @@
         <v>58.338999999999999</v>
       </c>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C47"/>
       <c r="D47"/>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>14</v>
       </c>
@@ -1007,21 +1013,21 @@
         <v>61.067999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>14</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D49">
         <v>62.542999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -1035,7 +1041,7 @@
         <v>48.273000000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -1043,13 +1049,13 @@
         <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E52" s="8">
         <v>48.585000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -1063,7 +1069,7 @@
         <v>48.780999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>24</v>
       </c>
@@ -1071,13 +1077,13 @@
         <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E54" s="8">
         <v>48.898000000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>24</v>
       </c>
@@ -1091,7 +1097,7 @@
         <v>50.468000000000004</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>24</v>
       </c>
@@ -1105,24 +1111,24 @@
         <v>51.713000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>25</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C58" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E58" s="8">
         <v>46.975000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D59" s="2"/>
     </row>
   </sheetData>

</xml_diff>